<commit_message>
add today status 18-12-2024
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jaya sri\A_Project_related\Daily status\Daily_Task_Status_\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jaya sri\A_Project_related\Daily_Status_\Daily_Task_Status_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05D95F5-FBCF-4F61-AE7E-799C9D4AFAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45867C2-65E2-4854-A07A-58B85C603349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>3.Some modifications in standup</t>
+  </si>
+  <si>
+    <t>login late tracker generation in tableau(sample file generation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheet preparation for leave tracker </t>
+  </si>
+  <si>
+    <t>ppt documents(3 sheets) ,2 incomplete</t>
   </si>
 </sst>
 </file>
@@ -153,14 +162,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,24 +468,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
@@ -489,7 +498,7 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>45636</v>
       </c>
       <c r="B3" t="s">
@@ -503,7 +512,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -512,7 +521,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -521,7 +530,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>45637</v>
       </c>
       <c r="B6" t="s">
@@ -532,7 +541,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -541,7 +550,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -550,7 +559,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -559,7 +568,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>45638</v>
       </c>
       <c r="B10" t="s">
@@ -573,7 +582,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -582,7 +591,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -591,7 +600,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -600,7 +609,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>45639</v>
       </c>
       <c r="B14" t="s">
@@ -611,7 +620,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -620,7 +629,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -629,7 +638,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -638,7 +647,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>45643</v>
       </c>
       <c r="B18" t="s">
@@ -652,7 +661,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -661,7 +670,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>26</v>
       </c>
@@ -670,7 +679,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -678,8 +687,47 @@
         <v>5</v>
       </c>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>45644</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A22:A25"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A9"/>

</xml_diff>